<commit_message>
Add Playwright tests for login form and various locators; include HTML structure and styles
</commit_message>
<xml_diff>
--- a/02.Examples/Database/Database Design & Questions.xlsx
+++ b/02.Examples/Database/Database Design & Questions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10315"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tony/GitHub/Aptech/tester-tutorials/02.Examples/Database/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F61624D-8152-0A44-9615-945D892F9448}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7810F19-1F59-E546-8F89-7B43A7DBB722}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="34560" windowHeight="19960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PHẦN I Tables" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="112">
   <si>
     <t>TABLE: Categories</t>
   </si>
@@ -367,6 +367,9 @@
   </si>
   <si>
     <t>AUTONUMBER / AUTO INCREMENT</t>
+  </si>
+  <si>
+    <t>ON UPDATE (CASCADE), ON DELETE(NO ACTION)</t>
   </si>
 </sst>
 </file>
@@ -1159,8 +1162,8 @@
   </sheetPr>
   <dimension ref="A1:AA883"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E31" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="I43" sqref="I43"/>
+    <sheetView tabSelected="1" topLeftCell="F42" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
+      <selection activeCell="J54" sqref="J54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1174,7 +1177,7 @@
     <col min="7" max="7" width="13.83203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15.1640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="39.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="29.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="43.83203125" customWidth="1"/>
     <col min="11" max="11" width="12.33203125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="22.1640625" bestFit="1" customWidth="1"/>
     <col min="13" max="27" width="10.5" customWidth="1"/>
@@ -3293,7 +3296,9 @@
       <c r="I56" s="61" t="s">
         <v>54</v>
       </c>
-      <c r="J56" s="61"/>
+      <c r="J56" s="61" t="s">
+        <v>111</v>
+      </c>
       <c r="K56" s="61"/>
       <c r="L56" s="61"/>
       <c r="M56" s="1"/>

</xml_diff>